<commit_message>
Updated Python Selenium Framework
</commit_message>
<xml_diff>
--- a/TestData/TestData.xlsx
+++ b/TestData/TestData.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PythonProjects\Selenium_Python_Framework\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBA43ACA-B157-44D3-A4F0-6F15A7BCEE6B}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AB1F940-BC46-4008-9905-328100499F6E}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoginModule" sheetId="1" r:id="rId1"/>
+    <sheet name="BookingModule" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="25">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -49,6 +50,57 @@
   </si>
   <si>
     <t>UserName</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>test_flightbooking</t>
+  </si>
+  <si>
+    <t>No_of_Passengers</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Departing_From</t>
+  </si>
+  <si>
+    <t>Departing_Day</t>
+  </si>
+  <si>
+    <t>Paris</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>Passenger_FirstName</t>
+  </si>
+  <si>
+    <t>Passenger_LastName</t>
+  </si>
+  <si>
+    <t>CreditCard_No</t>
+  </si>
+  <si>
+    <t>R</t>
+  </si>
+  <si>
+    <t>0123456789</t>
+  </si>
+  <si>
+    <t>Samrudh</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sandhya </t>
   </si>
 </sst>
 </file>
@@ -407,7 +459,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -450,7 +502,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>6</v>
@@ -470,11 +522,167 @@
         <v>6</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18652895-FFE4-4B1F-AEC1-D527729E879E}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J6" sqref="J6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="7.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>